<commit_message>
Fixed typos and add the average rank table
</commit_message>
<xml_diff>
--- a/results/NB.xlsx
+++ b/results/NB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PKW\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB9AC2C-CAD6-4044-874A-4F5180C9CB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0E869FF-B7F2-47D6-B3C6-FF01A57FAB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NB" sheetId="5" r:id="rId1"/>
@@ -122,14 +122,16 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,8 +156,14 @@
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -304,11 +312,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -398,6 +424,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,6 +444,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>787849</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>173170</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDE3FADD-DF5F-40F4-A485-D7D642CEB233}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11058525" y="91440"/>
+          <a:ext cx="6579049" cy="1481905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -619,7 +699,7 @@
   <dimension ref="A1:K46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -932,20 +1012,20 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="15"/>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="8">
-        <v>60</v>
-      </c>
-      <c r="D10" s="8">
+      <c r="C10" s="50">
+        <v>80</v>
+      </c>
+      <c r="D10" s="51">
         <v>67</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="47">
         <v>33</v>
       </c>
-      <c r="F10" s="4">
-        <v>42</v>
+      <c r="F10" s="49">
+        <v>43</v>
       </c>
       <c r="G10" s="8">
         <v>3</v>
@@ -968,16 +1048,16 @@
       <c r="B11" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="48">
         <v>80</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="48">
         <v>66</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="47">
         <v>31</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="4">
         <v>42</v>
       </c>
       <c r="G11" s="36">
@@ -2167,5 +2247,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>